<commit_message>
implemented password update and user deletion.
</commit_message>
<xml_diff>
--- a/src/main/resources/banco/senha/secrets.xlsx
+++ b/src/main/resources/banco/senha/secrets.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5f1b8306b924c59f/Programação/Java/ProjetosPessoais/LojaOnline/Login/SecureSignIn/src/main/resources/banco/senha/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="11_AD4D361C20488DEA4E38A0690C9D48425ADEDD87" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CE5FB2D-1EBF-482F-B3BE-7417DDDC1795}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="11_AD4D361C20488DEA4E38A0690C9D48425ADEDD87" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D15ED813-5F1E-460B-9EA0-7EFCB88B697F}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="senhas" sheetId="1" r:id="rId1"/>
+    <sheet name="BancoDeSenhas" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>userId</t>
   </si>
@@ -33,26 +34,65 @@
     <t>senhaHash</t>
   </si>
   <si>
-    <t>Salt</t>
-  </si>
-  <si>
     <t>createdDate</t>
   </si>
   <si>
     <t>lastUpdate</t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t>salt</t>
+  </si>
+  <si>
+    <t>userTest2</t>
+  </si>
+  <si>
+    <t>$2a$10$v6prcIuYAEe4.e108IkqPOISke.EDpT/56YDKtlJVR1qrXxjgemcC</t>
+  </si>
+  <si>
+    <t>$2a$10$v6prcIuYAEe4.e108IkqPO</t>
+  </si>
+  <si>
+    <t>2024-03-17T17:46:48.112927500</t>
+  </si>
+  <si>
+    <t>userTest1</t>
+  </si>
+  <si>
+    <t>$2a$10$Thq0gDRIqAUEeMr038QXtOpcRdjP2.tKo6gX5H/TqSnsX0EhYzKUe</t>
+  </si>
+  <si>
+    <t>$2a$10$Thq0gDRIqAUEeMr038QXtO</t>
+  </si>
+  <si>
+    <t>2024-03-17T17:48:36.397498700</t>
+  </si>
+  <si>
+    <t>$2a$10$yMQ4XLShIl6ocKan/tcihO4y6vhfBaDdhDsqpiJXurRlx4azdwoa2</t>
+  </si>
+  <si>
+    <t>$2a$10$yMQ4XLShIl6ocKan/tcihO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -63,7 +103,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -73,21 +113,49 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0"/>
+        <color theme="1"/>
       </left>
       <right style="thin">
-        <color theme="0"/>
+        <color theme="1"/>
       </right>
       <top style="thin">
-        <color theme="0"/>
+        <color theme="1"/>
       </top>
       <bottom style="thin">
-        <color theme="0"/>
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
       <right style="thin">
         <color theme="0"/>
       </right>
@@ -103,17 +171,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,25 +465,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="A2:XFD3"/>
+      <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.08984375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="62" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="32.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="28.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="28.08984375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.7265625" style="3" collapsed="1"/>
-    <col min="7" max="16384" width="8.7265625" style="2" collapsed="1"/>
+    <col min="1" max="1" width="15.7265625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="65" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="30.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="28.08984375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,18 +487,88 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="sZIpPAQ3TNlMGQc4q9R+XLjBpgpa8l50TJMU4MIIt3F2NgmbtlGcq1Zmhtd6cKWYjTPwrA860zuP/R4IbBgDdg==" saltValue="CDZhS3ILRFzUEbB9wUqOOg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A898F12-2498-4189-B601-A556F335F063}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="62.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>